<commit_message>
Got submission upload example working
</commit_message>
<xml_diff>
--- a/configuration/submission_templates/Pre-mixed.xlsx
+++ b/configuration/submission_templates/Pre-mixed.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrewss\git\sierra2\configuration\submission_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E201414-5122-463A-B54A-D10321B97899}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9309890C-6F15-4235-9570-2D851BB6A0AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{32635B5F-A8BA-47E0-ACF6-6DA028286940}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,16 +26,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>I'm a pre mixed library!!!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+  <si>
+    <t>Babraham Sequencing Facility Sample Sheet</t>
+  </si>
+  <si>
+    <t>Library Prep Type</t>
+  </si>
+  <si>
+    <t>Pre-mixed library</t>
+  </si>
+  <si>
+    <t>Sequencing Type</t>
+  </si>
+  <si>
+    <t>DON'T CHANGE ANYTHING ON THIS SHEET</t>
+  </si>
+  <si>
+    <t>NovaSeq 150bp PE</t>
+  </si>
+  <si>
+    <t>HiSeq 100bp SE</t>
+  </si>
+  <si>
+    <t>MiSeq 200bp SE</t>
+  </si>
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>Sample Type</t>
+  </si>
+  <si>
+    <t>10x-feature</t>
+  </si>
+  <si>
+    <t>rna-seq</t>
+  </si>
+  <si>
+    <t>chip-seq</t>
+  </si>
+  <si>
+    <t>10x-rna</t>
+  </si>
+  <si>
+    <t>5 Prime Barcode</t>
+  </si>
+  <si>
+    <t>3 Prime Barcode</t>
+  </si>
+  <si>
+    <t>Sample Number</t>
+  </si>
+  <si>
+    <t>Submission Name</t>
+  </si>
+  <si>
+    <t>Please fill in all of the yellow boxes</t>
+  </si>
+  <si>
+    <t>Fill in as many samples as you need.</t>
+  </si>
+  <si>
+    <t>Add more lines to the list of samples if there aren't enough</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +103,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -59,12 +156,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -80,6 +232,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1085850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Sequencing">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A7CDF7-12F3-4A4A-972F-9B817DA96816}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="152400" y="47625"/>
+          <a:ext cx="1038225" cy="1038225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,15 +597,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5221F4FC-85BD-4988-90C1-5357698C64AE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0"/>
+  <mergeCells count="4">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2EE0861A-E832-4D82-A8A6-9F9DE8BDB882}">
+          <x14:formula1>
+            <xm:f>Options!$A$3:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{965F35C9-288D-4BE1-9B2E-C47CBC21FCB0}">
+          <x14:formula1>
+            <xm:f>Options!$D$3:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDF77FD-CEE8-4AD0-81D6-6AB1A2EE8659}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>